<commit_message>
adding 2 metrics functions and file reader
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -348,22 +348,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1">
-        <v>1</v>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="B1">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="C1">
+        <v>0.01785714285714286</v>
       </c>
       <c r="D1">
-        <v>0.03115379770661638</v>
-      </c>
-      <c r="E1" t="b">
-        <v>1</v>
+        <v>0.01354488130552715</v>
       </c>
       <c r="F1">
         <v>1</v>
       </c>
       <c r="G1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1">
-        <v>0.507788449426654</v>
+        <v>0.2027089762611055</v>
       </c>
     </row>
   </sheetData>

</xml_diff>